<commit_message>
update scoring codes docs
</commit_message>
<xml_diff>
--- a/inst/extdata/longgold_scoring_codes.xlsx
+++ b/inst/extdata/longgold_scoring_codes.xlsx
@@ -1483,7 +1483,7 @@
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.5"/>
   </cols>
@@ -1862,7 +1862,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.38"/>
@@ -2070,10 +2070,10 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.25"/>
   </cols>
   <sheetData>
@@ -2260,7 +2260,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.62"/>
@@ -2789,7 +2789,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.5"/>
@@ -3037,7 +3037,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.62"/>
@@ -3225,7 +3225,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.87"/>
@@ -4225,7 +4225,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.63"/>
@@ -4552,9 +4552,9 @@
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5179,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.6"/>
@@ -5308,7 +5308,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.34"/>
@@ -5456,12 +5456,12 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5706,7 +5706,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -6257,7 +6257,7 @@
       <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
@@ -7227,9 +7227,9 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.5"/>
   </cols>
   <sheetData>
@@ -7393,7 +7393,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.38"/>
   </cols>
@@ -7940,9 +7940,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>